<commit_message>
lcn-ex/site: added rina-os, bug fixes
</commit_message>
<xml_diff>
--- a/src/main/lcn-examples/rina/complexity.xlsx
+++ b/src/main/lcn-examples/rina/complexity.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF8EA71-F053-40ED-A6CB-7F2DD37437AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C15B18-FEF3-48CE-88C3-28A545AF1B08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="rina" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">rina!$A$1:$L$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">rina!$A$1:$M$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>2H</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>SN WiFi</t>
+  </si>
+  <si>
+    <t>OS</t>
   </si>
 </sst>
 </file>
@@ -710,21 +713,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:K14"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="10.140625" customWidth="1"/>
-    <col min="12" max="12" width="1.7109375" customWidth="1"/>
+    <col min="3" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -737,8 +740,9 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -768,9 +772,12 @@
       <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -802,9 +809,12 @@
       <c r="K3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -836,9 +846,12 @@
       <c r="K4" s="14">
         <v>5</v>
       </c>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="14">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
         <v>17</v>
@@ -870,9 +883,12 @@
       <c r="K5" s="9">
         <v>1</v>
       </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="9">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="13" t="s">
         <v>26</v>
@@ -904,9 +920,12 @@
       <c r="K6" s="10">
         <v>4</v>
       </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="10">
+        <v>2</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="13" t="s">
         <v>18</v>
@@ -934,9 +953,12 @@
       <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
         <v>9</v>
@@ -946,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="14">
-        <f t="shared" ref="D8:K8" si="0">D5+D6+D7</f>
+        <f t="shared" ref="D8:L8" si="0">D5+D6+D7</f>
         <v>4</v>
       </c>
       <c r="E8" s="14">
@@ -977,9 +999,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12" t="s">
         <v>19</v>
@@ -1011,9 +1037,12 @@
       <c r="K9" s="9">
         <v>13</v>
       </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="9">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="13" t="s">
         <v>20</v>
@@ -1041,9 +1070,12 @@
       <c r="K10" s="10">
         <v>1</v>
       </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="10">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -1053,7 +1085,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="14">
-        <f t="shared" ref="D11:K11" si="1">D9+D10</f>
+        <f t="shared" ref="D11:L11" si="1">D9+D10</f>
         <v>9</v>
       </c>
       <c r="E11" s="14">
@@ -1084,9 +1116,13 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="L11" s="14">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
         <v>11</v>
@@ -1096,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" ref="D12:K12" si="2">D4+D8</f>
+        <f t="shared" ref="D12:L12" si="2">D4+D8</f>
         <v>7</v>
       </c>
       <c r="E12" s="9">
@@ -1124,12 +1160,16 @@
         <v>24</v>
       </c>
       <c r="K12" s="9">
+        <f t="shared" ref="K12" si="3">K4+K8</f>
+        <v>11</v>
+      </c>
+      <c r="L12" s="9">
         <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="6" t="s">
         <v>13</v>
@@ -1139,40 +1179,44 @@
         <v>9</v>
       </c>
       <c r="D13" s="10">
-        <f t="shared" ref="D13:K13" si="3">D8+D11</f>
+        <f t="shared" ref="D13:L13" si="4">D8+D11</f>
         <v>13</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="F13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="H13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="I13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33</v>
       </c>
       <c r="J13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
       <c r="K13" s="10">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="K13" si="5">K8+K11</f>
         <v>20</v>
       </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="L13" s="10">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="6" t="s">
         <v>12</v>
@@ -1182,40 +1226,44 @@
         <v>8</v>
       </c>
       <c r="D14" s="10">
-        <f t="shared" ref="D14:K14" si="4">D4+D11</f>
+        <f t="shared" ref="D14:L14" si="6">D4+D11</f>
         <v>12</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="F14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="H14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
       <c r="I14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
       <c r="J14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
       <c r="K14" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K14" si="7">K4+K11</f>
         <v>19</v>
       </c>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="10">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="4" t="s">
         <v>14</v>
@@ -1225,40 +1273,44 @@
         <v>11</v>
       </c>
       <c r="D15" s="14">
-        <f t="shared" ref="D15:K15" si="5">D4+D8+D11</f>
+        <f t="shared" ref="D15:L15" si="8">D4+D8+D11</f>
         <v>16</v>
       </c>
       <c r="E15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="F15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="G15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="H15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="I15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
       <c r="J15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="K15" s="14">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K15" si="9">K4+K8+K11</f>
         <v>25</v>
       </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="14">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="12" t="s">
         <v>32</v>
@@ -1290,9 +1342,12 @@
       <c r="K16" s="9">
         <v>8</v>
       </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="9">
+        <v>4</v>
+      </c>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="13" t="s">
         <v>33</v>
@@ -1324,9 +1379,12 @@
       <c r="K17" s="10">
         <v>4</v>
       </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="10">
+        <v>2</v>
+      </c>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="7" t="s">
         <v>15</v>
@@ -1336,40 +1394,44 @@
         <v>3</v>
       </c>
       <c r="D18" s="15">
-        <f t="shared" ref="D18:K18" si="6">D16+D17</f>
+        <f t="shared" ref="D18:L18" si="10">D16+D17</f>
         <v>6</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="F18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="G18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="H18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="I18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="J18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
       <c r="K18" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="K18" si="11">K16+K17</f>
         <v>12</v>
       </c>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="15">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="8" t="s">
         <v>16</v>
@@ -1379,40 +1441,44 @@
         <v>14</v>
       </c>
       <c r="D19" s="16">
-        <f t="shared" ref="D19:K19" si="7">D15+D18</f>
+        <f t="shared" ref="D19:L19" si="12">D15+D18</f>
         <v>22</v>
       </c>
       <c r="E19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>20</v>
       </c>
       <c r="F19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>28</v>
       </c>
       <c r="G19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>41</v>
       </c>
       <c r="H19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>65</v>
       </c>
       <c r="I19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>62</v>
       </c>
       <c r="J19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>79</v>
       </c>
       <c r="K19" s="16">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="K19" si="13">K15+K18</f>
         <v>37</v>
       </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="16">
+        <f t="shared" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="9" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1425,6 +1491,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>